<commit_message>
Update test resources for new frontend and namespace feature
</commit_message>
<xml_diff>
--- a/test/assets/project-administration/model/ProjectAdministration.xlsx
+++ b/test/assets/project-administration/model/ProjectAdministration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\ampersand-tarski\project-administration\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projecten\Ampersand\Project-administration-master\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F39260D-979B-43E2-B148-C4571574C416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427AA05A-7B27-4900-8151-E7C1D4A0CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Projects" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>Project</t>
   </si>
@@ -304,9 +304,6 @@
   </si>
   <si>
     <t>1970_13</t>
-  </si>
-  <si>
-    <t>[Members]</t>
   </si>
   <si>
     <t>workswith</t>
@@ -366,20 +363,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,9 +389,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -435,9 +429,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -470,26 +464,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,26 +499,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -717,23 +677,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="7" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -745,7 +706,7 @@
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -755,8 +716,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -768,33 +729,33 @@
       <c r="D2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>41639</v>
       </c>
-      <c r="F3" s="5" t="str">
+      <c r="F3" t="str">
         <f>A3</f>
         <v>2013_01</v>
       </c>
@@ -802,236 +763,229 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="5">
         <v>41685</v>
       </c>
-      <c r="F4" s="5" t="str">
+      <c r="F4" t="str">
         <f>A4</f>
         <v>2014_01</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>41835</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="5" t="str">
+      <c r="F7" t="str">
         <f>A7</f>
         <v>2014_05</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>25675</v>
       </c>
-      <c r="F8" s="5" t="str">
+      <c r="F8" t="str">
         <f>A8</f>
         <v>1970_13</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>91</v>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>85</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>85</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>85</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>86</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>86</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>86</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>87</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>87</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>90</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>90</v>
       </c>
       <c r="B24" t="s">
@@ -1048,21 +1002,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="17" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1077,15 +1032,15 @@
       <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1100,207 +1055,207 @@
       <c r="E2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>